<commit_message>
✏️ Update name of column to be validated
</commit_message>
<xml_diff>
--- a/tests/data/IG_POSICION_TRAMPAS_10MAY2020.xlsx
+++ b/tests/data/IG_POSICION_TRAMPAS_10MAY2020.xlsx
@@ -12,8 +12,8 @@
     <sheet name="Hoja1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">Coor-Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre del responsable</t>
+    <t xml:space="preserve">Nombre_del_responsable</t>
   </si>
   <si>
     <t xml:space="preserve">04//May/2020</t>
@@ -296,12 +296,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -393,7 +393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -402,13 +402,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
@@ -417,7 +416,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,16 +769,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K10"/>
+  <autoFilter ref="A1:K9"/>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A9">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -794,7 +788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -804,10 +798,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -963,19 +954,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A19">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C19">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>